<commit_message>
module html update 11/14
</commit_message>
<xml_diff>
--- a/opus-international-component-generator/표준폼필드목록.xlsx
+++ b/opus-international-component-generator/표준폼필드목록.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2000383\Documents\My Source\opus-international-component-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2915E08-1CF4-4749-A822-D292725D9D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF6C0BA-0EC8-414A-BE70-6BDBCFA36839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="1425" windowWidth="21180" windowHeight="12960" xr2:uid="{153749E0-B9B9-4FA3-9C24-72EF5ECB581F}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13320" windowHeight="13200" xr2:uid="{153749E0-B9B9-4FA3-9C24-72EF5ECB581F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="107">
   <si>
     <t>item type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -436,6 +436,30 @@
   </si>
   <si>
     <t xml:space="preserve">    &lt;i class="decrease"&gt;&lt;/i&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>focus/blur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read-only</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -443,7 +467,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,6 +478,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -482,11 +514,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,7 +841,7 @@
   <dimension ref="A2:P84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -814,12 +849,12 @@
     <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>18</v>
       </c>
@@ -838,8 +873,11 @@
       <c r="H3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -864,8 +902,11 @@
       <c r="H4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>19</v>
       </c>
@@ -873,7 +914,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -881,8 +922,11 @@
       <c r="H5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>30</v>
       </c>
@@ -890,7 +934,7 @@
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -898,37 +942,49 @@
       <c r="H6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
+      <c r="J6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -939,7 +995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -947,12 +1003,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>65</v>
       </c>

</xml_diff>